<commit_message>
1171. Fix fwdrerere, fwdfwd, rererere, fwdrerere.
</commit_message>
<xml_diff>
--- a/media/forUnitTests.xlsx
+++ b/media/forUnitTests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr backupFile="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="21840" windowHeight="13050" tabRatio="744" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="21840" windowHeight="13050" tabRatio="341" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Forma_1" sheetId="51" r:id="rId1"/>
@@ -25,7 +25,6 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Activities!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ALL DIALOGUES(E+T+RS+RV)'!$A$2:$ED$14</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'ALL Themes'!$A$1:$W$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Documents!$A$1:$N$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Faces_new!$A$1:$M$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Forma_1!$A$1:$F$1</definedName>
@@ -5333,7 +5332,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2145" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2176" uniqueCount="623">
   <si>
     <t>герой</t>
   </si>
@@ -6862,9 +6861,6 @@
     <t>Техническое поле</t>
   </si>
   <si>
-    <t>Проверка с F-S-C</t>
-  </si>
-  <si>
     <t>Original_Theme_id</t>
   </si>
   <si>
@@ -6877,13 +6873,7 @@
     <t>Prefix_text</t>
   </si>
   <si>
-    <t>Проверка с Mail_Inbox</t>
-  </si>
-  <si>
     <t>Theme_text</t>
-  </si>
-  <si>
-    <t>Проверка с Mail_Outbox</t>
   </si>
   <si>
     <t>Mail_code</t>
@@ -7311,6 +7301,54 @@
   </si>
   <si>
     <t>+7(926)720-0002</t>
+  </si>
+  <si>
+    <t>rere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re: Re: </t>
+  </si>
+  <si>
+    <t>Re: Re: обновление информации</t>
+  </si>
+  <si>
+    <t>Срочно жду бюджет логистики</t>
+  </si>
+  <si>
+    <t>rerere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re: Re: Re: </t>
+  </si>
+  <si>
+    <t>Егор Трудякин</t>
+  </si>
+  <si>
+    <t>Re: Re: Re: Срочно жду бюджет логистики</t>
+  </si>
+  <si>
+    <t>Начальник отдела логистики</t>
+  </si>
+  <si>
+    <t>Нач. логистики</t>
+  </si>
+  <si>
+    <t>trudyakin.ek@skiliks.com</t>
+  </si>
+  <si>
+    <t>trudyakin.ek</t>
+  </si>
+  <si>
+    <t>+7(926)720-1114</t>
+  </si>
+  <si>
+    <t>Проверка с F-S-C</t>
+  </si>
+  <si>
+    <t>Проверка с Mail_Inbox</t>
+  </si>
+  <si>
+    <t>Проверка с Mail_Outbox</t>
   </si>
 </sst>
 </file>
@@ -10318,7 +10356,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="588">
+  <cellXfs count="589">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -11487,6 +11525,219 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="58" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="43" xfId="1218" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="24" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="7" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="31" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="26" fillId="0" borderId="36" xfId="1218" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="36" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="36" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="52" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="22" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="47" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="41" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="36" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="36" xfId="1218" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="52" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="47" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="47" xfId="1218" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="52" xfId="1218" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="1218" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="66" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="70" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="1218" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="24" xfId="1218" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="43" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="50" xfId="1218" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="1218" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="52" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="26" fillId="0" borderId="56" xfId="1218" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="56" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="56" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="64" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="71" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="64" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="30" borderId="22" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="18" xfId="1218" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="61" xfId="1218" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="26" fillId="0" borderId="39" xfId="1218" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="39" xfId="1218" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="2" xfId="1218" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="39" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="39" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="65" xfId="1218" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="3" borderId="18" xfId="1218" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="29" xfId="1218" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="28" borderId="26" xfId="1218" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -11858,216 +12109,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="58" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="43" xfId="1218" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="24" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="7" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="31" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="26" fillId="0" borderId="36" xfId="1218" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="36" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="36" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="52" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="22" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="47" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="41" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="36" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="36" xfId="1218" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="52" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="47" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="47" xfId="1218" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="52" xfId="1218" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="1218" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="66" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="70" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="1218" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="24" xfId="1218" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="43" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="50" xfId="1218" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="1218" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="52" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="26" fillId="0" borderId="56" xfId="1218" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="56" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="56" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="64" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="71" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="64" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="30" borderId="22" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="18" xfId="1218" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="61" xfId="1218" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="26" fillId="0" borderId="39" xfId="1218" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="39" xfId="1218" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="2" xfId="1218" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="39" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="39" xfId="1218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="65" xfId="1218" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="3" borderId="18" xfId="1218" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="29" xfId="1218" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1627">
@@ -14221,19 +14262,19 @@
   <sheetData>
     <row r="1" spans="1:14" s="10" customFormat="1" ht="32.25" thickBot="1">
       <c r="A1" s="370" t="s">
+        <v>519</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>520</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>521</v>
+      </c>
+      <c r="D1" s="31" t="s">
         <v>522</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="E1" s="392" t="s">
         <v>523</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>524</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>525</v>
-      </c>
-      <c r="E1" s="392" t="s">
-        <v>526</v>
       </c>
       <c r="F1" s="375" t="s">
         <v>479</v>
@@ -14305,7 +14346,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="9" customFormat="1" ht="48" thickBot="1">
       <c r="A1" s="27" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B1" s="28" t="s">
         <v>499</v>
@@ -15300,14 +15341,14 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C17" sqref="C17"/>
       <selection pane="topRight" activeCell="C17" sqref="C17"/>
       <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
-      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -15449,16 +15490,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="318" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C4" s="318" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D4" s="85" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="E4" s="85" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F4" s="330">
         <v>8</v>
@@ -15473,16 +15514,16 @@
         <v>10</v>
       </c>
       <c r="J4" s="324" t="s">
+        <v>550</v>
+      </c>
+      <c r="K4" s="325" t="s">
+        <v>551</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>552</v>
+      </c>
+      <c r="M4" s="318" t="s">
         <v>553</v>
-      </c>
-      <c r="K4" s="325" t="s">
-        <v>554</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>555</v>
-      </c>
-      <c r="M4" s="318" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="16.5" customHeight="1">
@@ -15490,16 +15531,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="318" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C5" s="318" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="D5" s="85" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="E5" s="85" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="F5" s="330">
         <v>16</v>
@@ -15514,16 +15555,16 @@
         <v>10</v>
       </c>
       <c r="J5" s="324" t="s">
+        <v>557</v>
+      </c>
+      <c r="K5" s="325" t="s">
+        <v>558</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>559</v>
+      </c>
+      <c r="M5" s="318" t="s">
         <v>560</v>
-      </c>
-      <c r="K5" s="325" t="s">
-        <v>561</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>562</v>
-      </c>
-      <c r="M5" s="318" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="31.5">
@@ -15531,16 +15572,16 @@
         <v>10</v>
       </c>
       <c r="B6" s="318" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="C6" s="318" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="D6" s="319" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E6" s="319" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="F6" s="330">
         <v>47</v>
@@ -15555,13 +15596,13 @@
         <v>11</v>
       </c>
       <c r="J6" s="324" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="K6" s="325" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="M6" s="16"/>
     </row>
@@ -15570,16 +15611,16 @@
         <v>19</v>
       </c>
       <c r="B7" s="318" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="C7" s="318" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="D7" s="319" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="E7" s="319" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="F7" s="330">
         <v>23</v>
@@ -15594,13 +15635,13 @@
         <v>11</v>
       </c>
       <c r="J7" s="324" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="K7" s="325" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="M7" s="16"/>
     </row>
@@ -15609,16 +15650,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="318" t="s">
+        <v>600</v>
+      </c>
+      <c r="C8" s="318" t="s">
+        <v>601</v>
+      </c>
+      <c r="D8" s="85" t="s">
+        <v>602</v>
+      </c>
+      <c r="E8" s="85" t="s">
         <v>603</v>
-      </c>
-      <c r="C8" s="318" t="s">
-        <v>604</v>
-      </c>
-      <c r="D8" s="85" t="s">
-        <v>605</v>
-      </c>
-      <c r="E8" s="85" t="s">
-        <v>606</v>
       </c>
       <c r="F8" s="330">
         <v>32</v>
@@ -15633,15 +15674,54 @@
         <v>12</v>
       </c>
       <c r="J8" s="324" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="K8" s="325" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="M8" s="16"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="317">
+        <v>12</v>
+      </c>
+      <c r="B9" s="318" t="s">
+        <v>615</v>
+      </c>
+      <c r="C9" s="318" t="s">
+        <v>616</v>
+      </c>
+      <c r="D9" s="319" t="s">
+        <v>613</v>
+      </c>
+      <c r="E9" s="319" t="s">
+        <v>613</v>
+      </c>
+      <c r="F9" s="330">
+        <v>26</v>
+      </c>
+      <c r="G9" s="333">
+        <v>14</v>
+      </c>
+      <c r="H9" s="330">
+        <v>13</v>
+      </c>
+      <c r="I9" s="333">
+        <v>13</v>
+      </c>
+      <c r="J9" s="324" t="s">
+        <v>617</v>
+      </c>
+      <c r="K9" s="325" t="s">
+        <v>618</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>619</v>
+      </c>
+      <c r="M9" s="16"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M3"/>
@@ -15660,6 +15740,8 @@
     <hyperlink ref="K7" r:id="rId12" display="golts.fe@skiliks.com"/>
     <hyperlink ref="J8" r:id="rId13"/>
     <hyperlink ref="K8" r:id="rId14" display="dolgova.nt@skiliks.com"/>
+    <hyperlink ref="J9" r:id="rId15"/>
+    <hyperlink ref="K9" r:id="rId16" display="trudyakin.ek@skiliks.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -15850,166 +15932,166 @@
       <c r="AB1" s="109"/>
       <c r="AC1" s="109"/>
       <c r="AD1" s="109"/>
-      <c r="AE1" s="438" t="s">
+      <c r="AE1" s="509" t="s">
         <v>176</v>
       </c>
-      <c r="AF1" s="439"/>
-      <c r="AG1" s="440" t="s">
+      <c r="AF1" s="510"/>
+      <c r="AG1" s="511" t="s">
         <v>107</v>
       </c>
-      <c r="AH1" s="440"/>
-      <c r="AI1" s="440"/>
-      <c r="AJ1" s="440"/>
-      <c r="AK1" s="440"/>
-      <c r="AL1" s="440"/>
-      <c r="AM1" s="440"/>
-      <c r="AN1" s="441"/>
-      <c r="AO1" s="442" t="s">
+      <c r="AH1" s="511"/>
+      <c r="AI1" s="511"/>
+      <c r="AJ1" s="511"/>
+      <c r="AK1" s="511"/>
+      <c r="AL1" s="511"/>
+      <c r="AM1" s="511"/>
+      <c r="AN1" s="512"/>
+      <c r="AO1" s="513" t="s">
         <v>178</v>
       </c>
-      <c r="AP1" s="443"/>
-      <c r="AQ1" s="443"/>
-      <c r="AR1" s="443"/>
-      <c r="AS1" s="443"/>
-      <c r="AT1" s="443"/>
-      <c r="AU1" s="443"/>
-      <c r="AV1" s="424" t="s">
+      <c r="AP1" s="514"/>
+      <c r="AQ1" s="514"/>
+      <c r="AR1" s="514"/>
+      <c r="AS1" s="514"/>
+      <c r="AT1" s="514"/>
+      <c r="AU1" s="514"/>
+      <c r="AV1" s="495" t="s">
         <v>187</v>
       </c>
-      <c r="AW1" s="425"/>
-      <c r="AX1" s="425"/>
-      <c r="AY1" s="425"/>
-      <c r="AZ1" s="425"/>
-      <c r="BA1" s="425"/>
-      <c r="BB1" s="425"/>
-      <c r="BC1" s="425"/>
-      <c r="BD1" s="424" t="s">
+      <c r="AW1" s="496"/>
+      <c r="AX1" s="496"/>
+      <c r="AY1" s="496"/>
+      <c r="AZ1" s="496"/>
+      <c r="BA1" s="496"/>
+      <c r="BB1" s="496"/>
+      <c r="BC1" s="496"/>
+      <c r="BD1" s="495" t="s">
         <v>188</v>
       </c>
-      <c r="BE1" s="425"/>
-      <c r="BF1" s="425"/>
-      <c r="BG1" s="426"/>
-      <c r="BH1" s="427" t="s">
+      <c r="BE1" s="496"/>
+      <c r="BF1" s="496"/>
+      <c r="BG1" s="497"/>
+      <c r="BH1" s="498" t="s">
         <v>2</v>
       </c>
-      <c r="BI1" s="428"/>
-      <c r="BJ1" s="428"/>
-      <c r="BK1" s="428"/>
-      <c r="BL1" s="428"/>
-      <c r="BM1" s="429"/>
-      <c r="BN1" s="430"/>
-      <c r="BO1" s="431" t="s">
+      <c r="BI1" s="499"/>
+      <c r="BJ1" s="499"/>
+      <c r="BK1" s="499"/>
+      <c r="BL1" s="499"/>
+      <c r="BM1" s="500"/>
+      <c r="BN1" s="501"/>
+      <c r="BO1" s="502" t="s">
         <v>3</v>
       </c>
-      <c r="BP1" s="432"/>
-      <c r="BQ1" s="432"/>
-      <c r="BR1" s="433" t="s">
+      <c r="BP1" s="503"/>
+      <c r="BQ1" s="503"/>
+      <c r="BR1" s="504" t="s">
         <v>4</v>
       </c>
-      <c r="BS1" s="434"/>
-      <c r="BT1" s="434"/>
-      <c r="BU1" s="434"/>
-      <c r="BV1" s="434"/>
-      <c r="BW1" s="435"/>
-      <c r="BX1" s="435"/>
-      <c r="BY1" s="435"/>
-      <c r="BZ1" s="436" t="s">
+      <c r="BS1" s="505"/>
+      <c r="BT1" s="505"/>
+      <c r="BU1" s="505"/>
+      <c r="BV1" s="505"/>
+      <c r="BW1" s="506"/>
+      <c r="BX1" s="506"/>
+      <c r="BY1" s="506"/>
+      <c r="BZ1" s="507" t="s">
         <v>5</v>
       </c>
-      <c r="CA1" s="437"/>
-      <c r="CB1" s="398" t="s">
+      <c r="CA1" s="508"/>
+      <c r="CB1" s="469" t="s">
         <v>164</v>
       </c>
-      <c r="CC1" s="399"/>
-      <c r="CD1" s="400"/>
-      <c r="CE1" s="401" t="s">
+      <c r="CC1" s="470"/>
+      <c r="CD1" s="471"/>
+      <c r="CE1" s="472" t="s">
         <v>165</v>
       </c>
-      <c r="CF1" s="402"/>
-      <c r="CG1" s="403" t="s">
+      <c r="CF1" s="473"/>
+      <c r="CG1" s="474" t="s">
         <v>6</v>
       </c>
-      <c r="CH1" s="404"/>
-      <c r="CI1" s="405"/>
-      <c r="CJ1" s="406" t="s">
+      <c r="CH1" s="475"/>
+      <c r="CI1" s="476"/>
+      <c r="CJ1" s="477" t="s">
         <v>166</v>
       </c>
-      <c r="CK1" s="407"/>
-      <c r="CL1" s="407"/>
-      <c r="CM1" s="408" t="s">
+      <c r="CK1" s="478"/>
+      <c r="CL1" s="478"/>
+      <c r="CM1" s="479" t="s">
         <v>167</v>
       </c>
-      <c r="CN1" s="409"/>
-      <c r="CO1" s="409"/>
-      <c r="CP1" s="410" t="s">
+      <c r="CN1" s="480"/>
+      <c r="CO1" s="480"/>
+      <c r="CP1" s="481" t="s">
         <v>168</v>
       </c>
-      <c r="CQ1" s="411"/>
-      <c r="CR1" s="411"/>
-      <c r="CS1" s="411"/>
-      <c r="CT1" s="411"/>
-      <c r="CU1" s="414" t="s">
+      <c r="CQ1" s="482"/>
+      <c r="CR1" s="482"/>
+      <c r="CS1" s="482"/>
+      <c r="CT1" s="482"/>
+      <c r="CU1" s="485" t="s">
         <v>169</v>
       </c>
-      <c r="CV1" s="415"/>
-      <c r="CW1" s="416"/>
-      <c r="CX1" s="417" t="s">
+      <c r="CV1" s="486"/>
+      <c r="CW1" s="487"/>
+      <c r="CX1" s="488" t="s">
         <v>170</v>
       </c>
-      <c r="CY1" s="418"/>
-      <c r="CZ1" s="418"/>
-      <c r="DA1" s="419"/>
-      <c r="DB1" s="419"/>
-      <c r="DC1" s="419"/>
-      <c r="DD1" s="420"/>
-      <c r="DE1" s="421" t="s">
+      <c r="CY1" s="489"/>
+      <c r="CZ1" s="489"/>
+      <c r="DA1" s="490"/>
+      <c r="DB1" s="490"/>
+      <c r="DC1" s="490"/>
+      <c r="DD1" s="491"/>
+      <c r="DE1" s="492" t="s">
         <v>198</v>
       </c>
-      <c r="DF1" s="422"/>
-      <c r="DG1" s="394" t="s">
+      <c r="DF1" s="493"/>
+      <c r="DG1" s="465" t="s">
         <v>199</v>
       </c>
-      <c r="DH1" s="423"/>
-      <c r="DI1" s="395"/>
-      <c r="DJ1" s="394" t="s">
+      <c r="DH1" s="494"/>
+      <c r="DI1" s="466"/>
+      <c r="DJ1" s="465" t="s">
         <v>7</v>
       </c>
-      <c r="DK1" s="395"/>
-      <c r="DL1" s="396" t="s">
+      <c r="DK1" s="466"/>
+      <c r="DL1" s="467" t="s">
         <v>171</v>
       </c>
-      <c r="DM1" s="397"/>
-      <c r="DN1" s="444" t="s">
+      <c r="DM1" s="468"/>
+      <c r="DN1" s="515" t="s">
         <v>172</v>
       </c>
-      <c r="DO1" s="445"/>
-      <c r="DP1" s="446"/>
+      <c r="DO1" s="516"/>
+      <c r="DP1" s="517"/>
       <c r="DQ1" s="111" t="s">
         <v>173</v>
       </c>
-      <c r="DR1" s="447" t="s">
+      <c r="DR1" s="518" t="s">
         <v>174</v>
       </c>
-      <c r="DS1" s="448"/>
-      <c r="DT1" s="449"/>
-      <c r="DU1" s="450" t="s">
+      <c r="DS1" s="519"/>
+      <c r="DT1" s="520"/>
+      <c r="DU1" s="521" t="s">
         <v>200</v>
       </c>
-      <c r="DV1" s="451"/>
-      <c r="DW1" s="451"/>
+      <c r="DV1" s="522"/>
+      <c r="DW1" s="522"/>
       <c r="DX1" s="112" t="s">
         <v>201</v>
       </c>
-      <c r="DY1" s="452" t="s">
+      <c r="DY1" s="523" t="s">
         <v>202</v>
       </c>
-      <c r="DZ1" s="453"/>
-      <c r="EA1" s="453"/>
-      <c r="EB1" s="454" t="s">
+      <c r="DZ1" s="524"/>
+      <c r="EA1" s="524"/>
+      <c r="EB1" s="525" t="s">
         <v>203</v>
       </c>
-      <c r="EC1" s="455"/>
-      <c r="ED1" s="456"/>
+      <c r="EC1" s="526"/>
+      <c r="ED1" s="527"/>
     </row>
     <row r="2" spans="1:134" ht="79.5" customHeight="1" thickBot="1">
       <c r="A2" s="113" t="s">
@@ -16031,7 +16113,7 @@
         <v>50</v>
       </c>
       <c r="G2" s="114" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="H2" s="115" t="s">
         <v>91</v>
@@ -16076,7 +16158,7 @@
         <v>97</v>
       </c>
       <c r="V2" s="114" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="W2" s="117" t="s">
         <v>455</v>
@@ -16090,10 +16172,10 @@
       <c r="Z2" s="336" t="s">
         <v>50</v>
       </c>
-      <c r="AA2" s="412" t="s">
+      <c r="AA2" s="483" t="s">
         <v>49</v>
       </c>
-      <c r="AB2" s="413"/>
+      <c r="AB2" s="484"/>
       <c r="AC2" s="337" t="s">
         <v>331</v>
       </c>
@@ -18671,8 +18753,8 @@
       <c r="G15" s="200" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="530" t="s">
-        <v>582</v>
+      <c r="H15" s="406" t="s">
+        <v>579</v>
       </c>
       <c r="I15" s="202"/>
       <c r="J15" s="203"/>
@@ -18689,19 +18771,19 @@
         <v>4</v>
       </c>
       <c r="O15" s="204" t="s">
-        <v>583</v>
-      </c>
-      <c r="P15" s="531" t="s">
+        <v>580</v>
+      </c>
+      <c r="P15" s="407" t="s">
         <v>98</v>
       </c>
-      <c r="Q15" s="531">
+      <c r="Q15" s="407">
         <v>1</v>
       </c>
-      <c r="R15" s="531">
+      <c r="R15" s="407">
         <v>1</v>
       </c>
-      <c r="S15" s="532" t="s">
-        <v>584</v>
+      <c r="S15" s="408" t="s">
+        <v>581</v>
       </c>
       <c r="T15" s="343">
         <v>39</v>
@@ -18709,11 +18791,11 @@
       <c r="U15" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="V15" s="533" t="s">
+      <c r="V15" s="409" t="s">
         <v>10</v>
       </c>
       <c r="W15" s="86" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="X15" s="86" t="e">
         <v>#N/A</v>
@@ -18832,31 +18914,31 @@
       <c r="ED15" s="220"/>
     </row>
     <row r="16" spans="1:134" ht="31.5">
-      <c r="A16" s="534">
+      <c r="A16" s="410">
         <v>32</v>
       </c>
-      <c r="B16" s="534">
+      <c r="B16" s="410">
         <v>32</v>
       </c>
-      <c r="C16" s="534" t="s">
+      <c r="C16" s="410" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="534" t="s">
+      <c r="D16" s="410" t="s">
         <v>456</v>
       </c>
-      <c r="E16" s="534" t="s">
+      <c r="E16" s="410" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="534">
+      <c r="F16" s="410">
         <v>1</v>
       </c>
       <c r="G16" s="266" t="s">
         <v>24</v>
       </c>
-      <c r="H16" s="535" t="s">
-        <v>582</v>
-      </c>
-      <c r="I16" s="536"/>
+      <c r="H16" s="411" t="s">
+        <v>579</v>
+      </c>
+      <c r="I16" s="412"/>
       <c r="J16" s="265"/>
       <c r="K16" s="96">
         <v>1</v>
@@ -18871,7 +18953,7 @@
         <v>4</v>
       </c>
       <c r="O16" s="267" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="P16" s="268" t="s">
         <v>98</v>
@@ -18882,32 +18964,32 @@
       <c r="R16" s="268">
         <v>2</v>
       </c>
-      <c r="S16" s="537" t="s">
-        <v>586</v>
-      </c>
-      <c r="T16" s="538">
+      <c r="S16" s="413" t="s">
+        <v>583</v>
+      </c>
+      <c r="T16" s="414">
         <v>78</v>
       </c>
-      <c r="U16" s="539" t="s">
+      <c r="U16" s="415" t="s">
         <v>14</v>
       </c>
-      <c r="V16" s="540" t="s">
+      <c r="V16" s="416" t="s">
         <v>10</v>
       </c>
-      <c r="W16" s="541" t="s">
+      <c r="W16" s="417" t="s">
         <v>10</v>
       </c>
-      <c r="X16" s="541" t="e">
+      <c r="X16" s="417" t="e">
         <v>#N/A</v>
       </c>
-      <c r="Y16" s="541"/>
+      <c r="Y16" s="417"/>
       <c r="Z16" s="96" t="s">
         <v>55</v>
       </c>
       <c r="AA16" s="96"/>
-      <c r="AB16" s="539"/>
-      <c r="AC16" s="539"/>
-      <c r="AD16" s="539"/>
+      <c r="AB16" s="415"/>
+      <c r="AC16" s="415"/>
+      <c r="AD16" s="415"/>
       <c r="AE16" s="151"/>
       <c r="AF16" s="152"/>
       <c r="AG16" s="153"/>
@@ -18937,81 +19019,81 @@
       <c r="BE16" s="156"/>
       <c r="BF16" s="156"/>
       <c r="BG16" s="156"/>
-      <c r="BH16" s="542"/>
-      <c r="BI16" s="543"/>
-      <c r="BJ16" s="543"/>
-      <c r="BK16" s="544"/>
-      <c r="BL16" s="543"/>
-      <c r="BM16" s="545"/>
-      <c r="BN16" s="546"/>
-      <c r="BO16" s="547"/>
-      <c r="BP16" s="543"/>
-      <c r="BQ16" s="543"/>
-      <c r="BR16" s="542"/>
-      <c r="BS16" s="543"/>
-      <c r="BT16" s="543"/>
-      <c r="BU16" s="543"/>
-      <c r="BV16" s="545"/>
-      <c r="BW16" s="543"/>
-      <c r="BX16" s="543"/>
-      <c r="BY16" s="543"/>
-      <c r="BZ16" s="542"/>
-      <c r="CA16" s="546"/>
-      <c r="CB16" s="548"/>
-      <c r="CC16" s="544"/>
-      <c r="CD16" s="549"/>
-      <c r="CE16" s="542"/>
-      <c r="CF16" s="543"/>
-      <c r="CG16" s="550"/>
-      <c r="CH16" s="547"/>
-      <c r="CI16" s="545"/>
-      <c r="CJ16" s="542"/>
-      <c r="CK16" s="544"/>
-      <c r="CL16" s="544"/>
-      <c r="CM16" s="547"/>
-      <c r="CN16" s="543"/>
-      <c r="CO16" s="543"/>
-      <c r="CP16" s="542"/>
-      <c r="CQ16" s="543"/>
-      <c r="CR16" s="544"/>
-      <c r="CS16" s="543"/>
-      <c r="CT16" s="550"/>
-      <c r="CU16" s="542"/>
-      <c r="CV16" s="543"/>
-      <c r="CW16" s="546"/>
-      <c r="CX16" s="547"/>
-      <c r="CY16" s="543"/>
-      <c r="CZ16" s="543"/>
-      <c r="DA16" s="545"/>
-      <c r="DB16" s="545"/>
-      <c r="DC16" s="545"/>
-      <c r="DD16" s="546"/>
-      <c r="DE16" s="547"/>
-      <c r="DF16" s="551"/>
-      <c r="DG16" s="542"/>
-      <c r="DH16" s="547"/>
-      <c r="DI16" s="552"/>
-      <c r="DJ16" s="543"/>
-      <c r="DK16" s="545"/>
-      <c r="DL16" s="542"/>
-      <c r="DM16" s="543"/>
-      <c r="DN16" s="547"/>
-      <c r="DO16" s="543"/>
-      <c r="DP16" s="545"/>
-      <c r="DQ16" s="542"/>
-      <c r="DR16" s="547"/>
-      <c r="DS16" s="543"/>
-      <c r="DT16" s="545"/>
-      <c r="DU16" s="542"/>
-      <c r="DV16" s="543"/>
-      <c r="DW16" s="543"/>
-      <c r="DX16" s="548"/>
-      <c r="DY16" s="542"/>
-      <c r="DZ16" s="543"/>
-      <c r="EA16" s="547"/>
-      <c r="EB16" s="547"/>
-      <c r="EC16" s="551"/>
-      <c r="ED16" s="546"/>
+      <c r="BH16" s="418"/>
+      <c r="BI16" s="419"/>
+      <c r="BJ16" s="419"/>
+      <c r="BK16" s="420"/>
+      <c r="BL16" s="419"/>
+      <c r="BM16" s="421"/>
+      <c r="BN16" s="422"/>
+      <c r="BO16" s="423"/>
+      <c r="BP16" s="419"/>
+      <c r="BQ16" s="419"/>
+      <c r="BR16" s="418"/>
+      <c r="BS16" s="419"/>
+      <c r="BT16" s="419"/>
+      <c r="BU16" s="419"/>
+      <c r="BV16" s="421"/>
+      <c r="BW16" s="419"/>
+      <c r="BX16" s="419"/>
+      <c r="BY16" s="419"/>
+      <c r="BZ16" s="418"/>
+      <c r="CA16" s="422"/>
+      <c r="CB16" s="424"/>
+      <c r="CC16" s="420"/>
+      <c r="CD16" s="425"/>
+      <c r="CE16" s="418"/>
+      <c r="CF16" s="419"/>
+      <c r="CG16" s="426"/>
+      <c r="CH16" s="423"/>
+      <c r="CI16" s="421"/>
+      <c r="CJ16" s="418"/>
+      <c r="CK16" s="420"/>
+      <c r="CL16" s="420"/>
+      <c r="CM16" s="423"/>
+      <c r="CN16" s="419"/>
+      <c r="CO16" s="419"/>
+      <c r="CP16" s="418"/>
+      <c r="CQ16" s="419"/>
+      <c r="CR16" s="420"/>
+      <c r="CS16" s="419"/>
+      <c r="CT16" s="426"/>
+      <c r="CU16" s="418"/>
+      <c r="CV16" s="419"/>
+      <c r="CW16" s="422"/>
+      <c r="CX16" s="423"/>
+      <c r="CY16" s="419"/>
+      <c r="CZ16" s="419"/>
+      <c r="DA16" s="421"/>
+      <c r="DB16" s="421"/>
+      <c r="DC16" s="421"/>
+      <c r="DD16" s="422"/>
+      <c r="DE16" s="423"/>
+      <c r="DF16" s="427"/>
+      <c r="DG16" s="418"/>
+      <c r="DH16" s="423"/>
+      <c r="DI16" s="428"/>
+      <c r="DJ16" s="419"/>
+      <c r="DK16" s="421"/>
+      <c r="DL16" s="418"/>
+      <c r="DM16" s="419"/>
+      <c r="DN16" s="423"/>
+      <c r="DO16" s="419"/>
+      <c r="DP16" s="421"/>
+      <c r="DQ16" s="418"/>
+      <c r="DR16" s="423"/>
+      <c r="DS16" s="419"/>
+      <c r="DT16" s="421"/>
+      <c r="DU16" s="418"/>
+      <c r="DV16" s="419"/>
+      <c r="DW16" s="419"/>
+      <c r="DX16" s="424"/>
+      <c r="DY16" s="418"/>
+      <c r="DZ16" s="419"/>
+      <c r="EA16" s="423"/>
+      <c r="EB16" s="423"/>
+      <c r="EC16" s="427"/>
+      <c r="ED16" s="422"/>
     </row>
     <row r="17" spans="1:134" ht="32.25" thickBot="1">
       <c r="A17" s="59">
@@ -19020,23 +19102,23 @@
       <c r="B17" s="59">
         <v>33</v>
       </c>
-      <c r="C17" s="534" t="s">
+      <c r="C17" s="410" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="534" t="s">
+      <c r="D17" s="410" t="s">
         <v>456</v>
       </c>
-      <c r="E17" s="534" t="s">
+      <c r="E17" s="410" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="534">
+      <c r="F17" s="410">
         <v>1</v>
       </c>
       <c r="G17" s="227" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="553" t="s">
-        <v>582</v>
+      <c r="H17" s="429" t="s">
+        <v>579</v>
       </c>
       <c r="I17" s="229"/>
       <c r="J17" s="230"/>
@@ -19053,7 +19135,7 @@
         <v>4</v>
       </c>
       <c r="O17" s="267" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="P17" s="268" t="s">
         <v>98</v>
@@ -19065,15 +19147,15 @@
         <v>3</v>
       </c>
       <c r="S17" s="172" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="T17" s="341">
         <v>53</v>
       </c>
-      <c r="U17" s="539" t="s">
+      <c r="U17" s="415" t="s">
         <v>14</v>
       </c>
-      <c r="V17" s="540" t="s">
+      <c r="V17" s="416" t="s">
         <v>10</v>
       </c>
       <c r="W17" s="87" t="s">
@@ -19196,31 +19278,31 @@
       <c r="ED17" s="243"/>
     </row>
     <row r="18" spans="1:134" ht="63.75" thickBot="1">
-      <c r="A18" s="575">
+      <c r="A18" s="451">
         <v>466</v>
       </c>
-      <c r="B18" s="575">
+      <c r="B18" s="451">
         <v>437</v>
       </c>
-      <c r="C18" s="575" t="s">
+      <c r="C18" s="451" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="575" t="s">
+      <c r="D18" s="451" t="s">
         <v>456</v>
       </c>
-      <c r="E18" s="575" t="s">
+      <c r="E18" s="451" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="575">
+      <c r="F18" s="451">
         <v>1</v>
       </c>
-      <c r="G18" s="576" t="s">
+      <c r="G18" s="452" t="s">
         <v>87</v>
       </c>
-      <c r="H18" s="577" t="s">
-        <v>588</v>
-      </c>
-      <c r="I18" s="578"/>
+      <c r="H18" s="453" t="s">
+        <v>585</v>
+      </c>
+      <c r="I18" s="454"/>
       <c r="J18" s="303"/>
       <c r="K18" s="304">
         <v>2</v>
@@ -19228,50 +19310,50 @@
       <c r="L18" s="304" t="s">
         <v>11</v>
       </c>
-      <c r="M18" s="579" t="s">
+      <c r="M18" s="455" t="s">
+        <v>590</v>
+      </c>
+      <c r="N18" s="456">
+        <v>1</v>
+      </c>
+      <c r="O18" s="456" t="s">
+        <v>0</v>
+      </c>
+      <c r="P18" s="457" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q18" s="457">
+        <v>1</v>
+      </c>
+      <c r="R18" s="457">
+        <v>0</v>
+      </c>
+      <c r="S18" s="458" t="s">
+        <v>591</v>
+      </c>
+      <c r="T18" s="459">
+        <v>356</v>
+      </c>
+      <c r="U18" s="460" t="s">
+        <v>12</v>
+      </c>
+      <c r="V18" s="461" t="s">
+        <v>36</v>
+      </c>
+      <c r="W18" s="455" t="s">
+        <v>592</v>
+      </c>
+      <c r="X18" s="455" t="s">
         <v>593</v>
       </c>
-      <c r="N18" s="580">
-        <v>1</v>
-      </c>
-      <c r="O18" s="580" t="s">
-        <v>0</v>
-      </c>
-      <c r="P18" s="581" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q18" s="581">
-        <v>1</v>
-      </c>
-      <c r="R18" s="581">
-        <v>0</v>
-      </c>
-      <c r="S18" s="582" t="s">
-        <v>594</v>
-      </c>
-      <c r="T18" s="583">
-        <v>356</v>
-      </c>
-      <c r="U18" s="584" t="s">
-        <v>12</v>
-      </c>
-      <c r="V18" s="585" t="s">
-        <v>36</v>
-      </c>
-      <c r="W18" s="579" t="s">
-        <v>595</v>
-      </c>
-      <c r="X18" s="579" t="s">
-        <v>596</v>
-      </c>
-      <c r="Y18" s="579"/>
-      <c r="Z18" s="579" t="s">
+      <c r="Y18" s="455"/>
+      <c r="Z18" s="455" t="s">
         <v>52</v>
       </c>
-      <c r="AA18" s="579"/>
-      <c r="AB18" s="579"/>
-      <c r="AC18" s="579"/>
-      <c r="AD18" s="579"/>
+      <c r="AA18" s="455"/>
+      <c r="AB18" s="455"/>
+      <c r="AC18" s="455"/>
+      <c r="AD18" s="455"/>
       <c r="AE18" s="233"/>
       <c r="AF18" s="234"/>
       <c r="AG18" s="235"/>
@@ -19397,8 +19479,8 @@
       <c r="G19" s="200" t="s">
         <v>408</v>
       </c>
-      <c r="H19" s="554" t="s">
-        <v>588</v>
+      <c r="H19" s="430" t="s">
+        <v>585</v>
       </c>
       <c r="I19" s="202"/>
       <c r="J19" s="203">
@@ -19411,10 +19493,10 @@
         <v>11</v>
       </c>
       <c r="M19" s="104"/>
-      <c r="N19" s="555">
+      <c r="N19" s="431">
         <v>1</v>
       </c>
-      <c r="O19" s="555" t="s">
+      <c r="O19" s="431" t="s">
         <v>0</v>
       </c>
       <c r="P19" s="203"/>
@@ -19444,10 +19526,10 @@
       <c r="Z19" s="104" t="s">
         <v>51</v>
       </c>
-      <c r="AA19" s="556"/>
-      <c r="AB19" s="557"/>
-      <c r="AC19" s="558"/>
-      <c r="AD19" s="558"/>
+      <c r="AA19" s="432"/>
+      <c r="AB19" s="433"/>
+      <c r="AC19" s="434"/>
+      <c r="AD19" s="434"/>
       <c r="AE19" s="233"/>
       <c r="AF19" s="234"/>
       <c r="AG19" s="235"/>
@@ -19554,34 +19636,34 @@
       <c r="ED19" s="243"/>
     </row>
     <row r="20" spans="1:134" ht="31.5">
-      <c r="A20" s="534">
+      <c r="A20" s="410">
         <v>464</v>
       </c>
-      <c r="B20" s="534"/>
-      <c r="C20" s="534" t="s">
+      <c r="B20" s="410"/>
+      <c r="C20" s="410" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="534" t="s">
+      <c r="D20" s="410" t="s">
         <v>457</v>
       </c>
-      <c r="E20" s="534" t="s">
+      <c r="E20" s="410" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="534">
+      <c r="F20" s="410">
         <v>1</v>
       </c>
       <c r="G20" s="227" t="s">
         <v>408</v>
       </c>
-      <c r="H20" s="559" t="s">
-        <v>588</v>
+      <c r="H20" s="435" t="s">
+        <v>585</v>
       </c>
       <c r="I20" s="229"/>
       <c r="J20" s="230"/>
-      <c r="K20" s="560">
+      <c r="K20" s="436">
         <v>1</v>
       </c>
-      <c r="L20" s="560" t="s">
+      <c r="L20" s="436" t="s">
         <v>0</v>
       </c>
       <c r="M20" s="97"/>
@@ -19599,7 +19681,7 @@
         <v>1</v>
       </c>
       <c r="S20" s="172" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="T20" s="341">
         <v>8</v>
@@ -19607,7 +19689,7 @@
       <c r="U20" s="278" t="s">
         <v>12</v>
       </c>
-      <c r="V20" s="574" t="s">
+      <c r="V20" s="450" t="s">
         <v>87</v>
       </c>
       <c r="W20" s="96" t="s">
@@ -19618,10 +19700,10 @@
       <c r="Z20" s="96" t="s">
         <v>51</v>
       </c>
-      <c r="AA20" s="561"/>
-      <c r="AB20" s="562"/>
-      <c r="AC20" s="563"/>
-      <c r="AD20" s="563"/>
+      <c r="AA20" s="437"/>
+      <c r="AB20" s="438"/>
+      <c r="AC20" s="439"/>
+      <c r="AD20" s="439"/>
       <c r="AE20" s="233"/>
       <c r="AF20" s="234"/>
       <c r="AG20" s="235"/>
@@ -19730,34 +19812,34 @@
       <c r="ED20" s="243"/>
     </row>
     <row r="21" spans="1:134" ht="32.25" thickBot="1">
-      <c r="A21" s="564">
+      <c r="A21" s="440">
         <v>465</v>
       </c>
-      <c r="B21" s="564"/>
-      <c r="C21" s="564" t="s">
+      <c r="B21" s="440"/>
+      <c r="C21" s="440" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="564" t="s">
+      <c r="D21" s="440" t="s">
         <v>457</v>
       </c>
-      <c r="E21" s="564" t="s">
+      <c r="E21" s="440" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="564">
+      <c r="F21" s="440">
         <v>1</v>
       </c>
-      <c r="G21" s="573" t="s">
+      <c r="G21" s="449" t="s">
         <v>408</v>
       </c>
-      <c r="H21" s="559" t="s">
-        <v>588</v>
-      </c>
-      <c r="I21" s="565"/>
+      <c r="H21" s="435" t="s">
+        <v>585</v>
+      </c>
+      <c r="I21" s="441"/>
       <c r="J21" s="280"/>
-      <c r="K21" s="560">
+      <c r="K21" s="436">
         <v>1</v>
       </c>
-      <c r="L21" s="560" t="s">
+      <c r="L21" s="436" t="s">
         <v>0</v>
       </c>
       <c r="M21" s="270"/>
@@ -19774,17 +19856,17 @@
       <c r="R21" s="280">
         <v>2</v>
       </c>
-      <c r="S21" s="566" t="s">
-        <v>590</v>
-      </c>
-      <c r="T21" s="567">
+      <c r="S21" s="442" t="s">
+        <v>587</v>
+      </c>
+      <c r="T21" s="443">
         <v>11</v>
       </c>
-      <c r="U21" s="568" t="s">
+      <c r="U21" s="444" t="s">
         <v>12</v>
       </c>
       <c r="V21" s="281" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="W21" s="284" t="s">
         <v>10</v>
@@ -19794,10 +19876,10 @@
       <c r="Z21" s="284" t="s">
         <v>51</v>
       </c>
-      <c r="AA21" s="569"/>
-      <c r="AB21" s="570"/>
-      <c r="AC21" s="571"/>
-      <c r="AD21" s="571"/>
+      <c r="AA21" s="445"/>
+      <c r="AB21" s="446"/>
+      <c r="AC21" s="447"/>
+      <c r="AD21" s="447"/>
       <c r="AE21" s="233"/>
       <c r="AF21" s="234"/>
       <c r="AG21" s="235"/>
@@ -19906,29 +19988,29 @@
       <c r="ED21" s="243"/>
     </row>
     <row r="22" spans="1:134" ht="63">
-      <c r="A22" s="586">
+      <c r="A22" s="462">
         <v>426</v>
       </c>
-      <c r="B22" s="586">
+      <c r="B22" s="462">
         <v>400</v>
       </c>
-      <c r="C22" s="586" t="s">
+      <c r="C22" s="462" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="586" t="s">
+      <c r="D22" s="462" t="s">
         <v>456</v>
       </c>
-      <c r="E22" s="586" t="s">
+      <c r="E22" s="462" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="586">
+      <c r="F22" s="462">
         <v>1</v>
       </c>
       <c r="G22" s="273" t="s">
         <v>36</v>
       </c>
-      <c r="H22" s="587" t="s">
-        <v>597</v>
+      <c r="H22" s="463" t="s">
+        <v>594</v>
       </c>
       <c r="I22" s="202"/>
       <c r="J22" s="203">
@@ -19938,10 +20020,10 @@
         <v>7</v>
       </c>
       <c r="L22" s="104" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="M22" s="104" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="N22" s="204">
         <v>1</v>
@@ -19958,8 +20040,8 @@
       <c r="R22" s="204">
         <v>0</v>
       </c>
-      <c r="S22" s="532" t="s">
-        <v>600</v>
+      <c r="S22" s="408" t="s">
+        <v>597</v>
       </c>
       <c r="T22" s="343">
         <v>87</v>
@@ -19971,10 +20053,10 @@
         <v>10</v>
       </c>
       <c r="W22" s="86" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="X22" s="86" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="Y22" s="86"/>
       <c r="Z22" s="104" t="s">
@@ -20090,8 +20172,8 @@
       <c r="ED22" s="243"/>
     </row>
     <row r="23" spans="1:134">
-      <c r="B23" s="572" t="s">
-        <v>592</v>
+      <c r="B23" s="448" t="s">
+        <v>589</v>
       </c>
     </row>
   </sheetData>
@@ -33395,19 +33477,19 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:W8"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomRight" activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="6.625" style="49" customWidth="1"/>
-    <col min="2" max="2" width="44.625" style="53" customWidth="1"/>
+    <col min="2" max="2" width="25" style="53" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.875" style="49" customWidth="1"/>
     <col min="6" max="6" width="9.375" customWidth="1"/>
@@ -33418,7 +33500,8 @@
     <col min="11" max="11" width="13.5" customWidth="1"/>
     <col min="12" max="12" width="22.125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="15" width="16.875" customWidth="1"/>
+    <col min="14" max="14" width="16.875" customWidth="1"/>
+    <col min="15" max="15" width="7.5" customWidth="1"/>
     <col min="16" max="16" width="56.5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="54.625" hidden="1" customWidth="1"/>
     <col min="18" max="19" width="39.125" hidden="1" customWidth="1"/>
@@ -33428,33 +33511,33 @@
     <col min="23" max="23" width="12.875" style="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="10" customFormat="1" ht="48" thickBot="1">
+    <row r="1" spans="1:23" ht="48" thickBot="1">
       <c r="A1" s="379" t="s">
+        <v>501</v>
+      </c>
+      <c r="B1" s="389" t="s">
         <v>502</v>
-      </c>
-      <c r="B1" s="389" t="s">
-        <v>503</v>
       </c>
       <c r="C1" s="390" t="s">
         <v>498</v>
       </c>
       <c r="D1" s="372" t="s">
+        <v>503</v>
+      </c>
+      <c r="E1" s="390" t="s">
         <v>504</v>
       </c>
-      <c r="E1" s="390" t="s">
-        <v>505</v>
-      </c>
       <c r="F1" s="374" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="G1" s="390" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="H1" s="372" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="I1" s="390" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="J1" s="390" t="s">
         <v>439</v>
@@ -33478,460 +33561,573 @@
         <v>500</v>
       </c>
       <c r="Q1" s="10" t="s">
+        <v>620</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>621</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="T1" s="379" t="s">
         <v>501</v>
       </c>
-      <c r="R1" s="10" t="s">
-        <v>506</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>508</v>
-      </c>
-      <c r="T1" s="379" t="s">
+      <c r="U1" s="389" t="s">
         <v>502</v>
-      </c>
-      <c r="U1" s="389" t="s">
-        <v>503</v>
       </c>
       <c r="V1" s="390" t="s">
         <v>498</v>
       </c>
       <c r="W1" s="390" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" s="11" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="518">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" s="394">
         <v>12</v>
       </c>
-      <c r="B2" s="519" t="s">
+      <c r="B2" s="395" t="s">
+        <v>528</v>
+      </c>
+      <c r="C2" s="396" t="s">
+        <v>529</v>
+      </c>
+      <c r="D2" s="397" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="398"/>
+      <c r="F2" s="399">
+        <v>10</v>
+      </c>
+      <c r="G2" s="400" t="s">
+        <v>530</v>
+      </c>
+      <c r="H2" s="401"/>
+      <c r="I2" s="402"/>
+      <c r="J2" s="396"/>
+      <c r="K2" s="396"/>
+      <c r="L2" s="399" t="s">
         <v>531</v>
       </c>
-      <c r="C2" s="520" t="s">
-        <v>532</v>
-      </c>
-      <c r="D2" s="521" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="522"/>
-      <c r="F2" s="523">
-        <v>10</v>
-      </c>
-      <c r="G2" s="524" t="s">
-        <v>533</v>
-      </c>
-      <c r="H2" s="525"/>
-      <c r="I2" s="526"/>
-      <c r="J2" s="520"/>
-      <c r="K2" s="520"/>
-      <c r="L2" s="523" t="s">
-        <v>534</v>
-      </c>
-      <c r="M2" s="525"/>
-      <c r="N2" s="525"/>
-      <c r="O2" s="527"/>
+      <c r="M2" s="401"/>
+      <c r="N2" s="401"/>
+      <c r="O2" s="403"/>
       <c r="P2" s="11" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="Q2" s="11" t="e">
         <v>#N/A</v>
       </c>
       <c r="R2" s="11" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="S2" s="11" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T2" s="518">
+      <c r="T2" s="394">
         <v>12</v>
       </c>
-      <c r="U2" s="519" t="s">
-        <v>531</v>
-      </c>
-      <c r="V2" s="520" t="s">
+      <c r="U2" s="395" t="s">
+        <v>528</v>
+      </c>
+      <c r="V2" s="396" t="s">
+        <v>529</v>
+      </c>
+      <c r="W2" s="398" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3" s="394">
+        <v>12</v>
+      </c>
+      <c r="B3" s="395" t="s">
+        <v>528</v>
+      </c>
+      <c r="C3" s="396" t="s">
         <v>532</v>
       </c>
-      <c r="W2" s="522" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" s="11" customFormat="1">
-      <c r="A3" s="518">
-        <v>12</v>
-      </c>
-      <c r="B3" s="519" t="s">
-        <v>531</v>
-      </c>
-      <c r="C3" s="520" t="s">
+      <c r="D3" s="397" t="s">
+        <v>533</v>
+      </c>
+      <c r="E3" s="398" t="s">
+        <v>534</v>
+      </c>
+      <c r="F3" s="399">
+        <v>1</v>
+      </c>
+      <c r="G3" s="400" t="s">
+        <v>447</v>
+      </c>
+      <c r="H3" s="397">
+        <v>3</v>
+      </c>
+      <c r="I3" s="402" t="s">
         <v>535</v>
       </c>
-      <c r="D3" s="521" t="s">
+      <c r="J3" s="398"/>
+      <c r="K3" s="398"/>
+      <c r="L3" s="399" t="s">
         <v>536</v>
       </c>
-      <c r="E3" s="522" t="s">
+      <c r="M3" s="397" t="s">
         <v>537</v>
       </c>
-      <c r="F3" s="523">
-        <v>1</v>
-      </c>
-      <c r="G3" s="524" t="s">
-        <v>447</v>
-      </c>
-      <c r="H3" s="521">
-        <v>3</v>
-      </c>
-      <c r="I3" s="526" t="s">
+      <c r="N3" s="397" t="s">
         <v>538</v>
       </c>
-      <c r="J3" s="522"/>
-      <c r="K3" s="522"/>
-      <c r="L3" s="523" t="s">
+      <c r="O3" s="404"/>
+      <c r="P3" s="11" t="s">
         <v>539</v>
       </c>
-      <c r="M3" s="521" t="s">
-        <v>540</v>
-      </c>
-      <c r="N3" s="521" t="s">
-        <v>541</v>
-      </c>
-      <c r="O3" s="528"/>
-      <c r="P3" s="11" t="s">
-        <v>542</v>
-      </c>
       <c r="Q3" s="11" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="R3" s="11" t="e">
         <v>#N/A</v>
       </c>
       <c r="S3" s="11" t="s">
+        <v>539</v>
+      </c>
+      <c r="T3" s="394">
+        <v>12</v>
+      </c>
+      <c r="U3" s="395" t="s">
+        <v>528</v>
+      </c>
+      <c r="V3" s="396" t="s">
+        <v>532</v>
+      </c>
+      <c r="W3" s="398" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4" s="394">
+        <v>12</v>
+      </c>
+      <c r="B4" s="395" t="s">
+        <v>528</v>
+      </c>
+      <c r="C4" s="396" t="s">
+        <v>532</v>
+      </c>
+      <c r="D4" s="397" t="s">
+        <v>533</v>
+      </c>
+      <c r="E4" s="398" t="s">
+        <v>534</v>
+      </c>
+      <c r="F4" s="399">
+        <v>1</v>
+      </c>
+      <c r="G4" s="400" t="s">
+        <v>447</v>
+      </c>
+      <c r="H4" s="397">
+        <v>4</v>
+      </c>
+      <c r="I4" s="402" t="s">
+        <v>540</v>
+      </c>
+      <c r="J4" s="398"/>
+      <c r="K4" s="398"/>
+      <c r="L4" s="399" t="s">
+        <v>541</v>
+      </c>
+      <c r="M4" s="397" t="s">
+        <v>537</v>
+      </c>
+      <c r="N4" s="397" t="s">
+        <v>538</v>
+      </c>
+      <c r="O4" s="404"/>
+      <c r="P4" s="11" t="s">
         <v>542</v>
       </c>
-      <c r="T3" s="518">
-        <v>12</v>
-      </c>
-      <c r="U3" s="519" t="s">
-        <v>531</v>
-      </c>
-      <c r="V3" s="520" t="s">
-        <v>535</v>
-      </c>
-      <c r="W3" s="522" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" s="11" customFormat="1">
-      <c r="A4" s="518">
-        <v>12</v>
-      </c>
-      <c r="B4" s="519" t="s">
-        <v>531</v>
-      </c>
-      <c r="C4" s="520" t="s">
-        <v>535</v>
-      </c>
-      <c r="D4" s="521" t="s">
-        <v>536</v>
-      </c>
-      <c r="E4" s="522" t="s">
-        <v>537</v>
-      </c>
-      <c r="F4" s="523">
-        <v>1</v>
-      </c>
-      <c r="G4" s="524" t="s">
-        <v>447</v>
-      </c>
-      <c r="H4" s="521">
-        <v>4</v>
-      </c>
-      <c r="I4" s="526" t="s">
-        <v>543</v>
-      </c>
-      <c r="J4" s="522"/>
-      <c r="K4" s="522"/>
-      <c r="L4" s="523" t="s">
-        <v>544</v>
-      </c>
-      <c r="M4" s="521" t="s">
-        <v>540</v>
-      </c>
-      <c r="N4" s="521" t="s">
-        <v>541</v>
-      </c>
-      <c r="O4" s="528"/>
-      <c r="P4" s="11" t="s">
-        <v>545</v>
-      </c>
       <c r="Q4" s="11" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="R4" s="11" t="e">
         <v>#N/A</v>
       </c>
       <c r="S4" s="11" t="s">
+        <v>542</v>
+      </c>
+      <c r="T4" s="394">
+        <v>12</v>
+      </c>
+      <c r="U4" s="395" t="s">
+        <v>528</v>
+      </c>
+      <c r="V4" s="396" t="s">
+        <v>532</v>
+      </c>
+      <c r="W4" s="398" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5" s="394">
+        <v>12</v>
+      </c>
+      <c r="B5" s="395" t="s">
+        <v>528</v>
+      </c>
+      <c r="C5" s="396" t="s">
+        <v>532</v>
+      </c>
+      <c r="D5" s="397" t="s">
+        <v>543</v>
+      </c>
+      <c r="E5" s="398" t="s">
+        <v>544</v>
+      </c>
+      <c r="F5" s="399">
+        <v>1</v>
+      </c>
+      <c r="G5" s="400" t="s">
+        <v>447</v>
+      </c>
+      <c r="H5" s="397">
+        <v>10</v>
+      </c>
+      <c r="I5" s="402" t="s">
+        <v>530</v>
+      </c>
+      <c r="J5" s="398"/>
+      <c r="K5" s="398"/>
+      <c r="L5" s="399" t="s">
         <v>545</v>
       </c>
-      <c r="T4" s="518">
-        <v>12</v>
-      </c>
-      <c r="U4" s="519" t="s">
-        <v>531</v>
-      </c>
-      <c r="V4" s="520" t="s">
-        <v>535</v>
-      </c>
-      <c r="W4" s="522" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" s="11" customFormat="1">
-      <c r="A5" s="518">
-        <v>12</v>
-      </c>
-      <c r="B5" s="519" t="s">
-        <v>531</v>
-      </c>
-      <c r="C5" s="520" t="s">
-        <v>535</v>
-      </c>
-      <c r="D5" s="521" t="s">
+      <c r="M5" s="397" t="s">
+        <v>537</v>
+      </c>
+      <c r="N5" s="397" t="s">
+        <v>294</v>
+      </c>
+      <c r="O5" s="404"/>
+      <c r="P5" s="11" t="s">
         <v>546</v>
       </c>
-      <c r="E5" s="522" t="s">
-        <v>547</v>
-      </c>
-      <c r="F5" s="523">
-        <v>1</v>
-      </c>
-      <c r="G5" s="524" t="s">
-        <v>447</v>
-      </c>
-      <c r="H5" s="521">
-        <v>10</v>
-      </c>
-      <c r="I5" s="526" t="s">
-        <v>533</v>
-      </c>
-      <c r="J5" s="522"/>
-      <c r="K5" s="522"/>
-      <c r="L5" s="523" t="s">
-        <v>548</v>
-      </c>
-      <c r="M5" s="521" t="s">
-        <v>540</v>
-      </c>
-      <c r="N5" s="521" t="s">
-        <v>294</v>
-      </c>
-      <c r="O5" s="528"/>
-      <c r="P5" s="11" t="s">
-        <v>549</v>
-      </c>
       <c r="Q5" s="11" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="R5" s="11" t="e">
         <v>#N/A</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>550</v>
-      </c>
-      <c r="T5" s="518">
+        <v>547</v>
+      </c>
+      <c r="T5" s="394">
         <v>12</v>
       </c>
-      <c r="U5" s="519" t="s">
+      <c r="U5" s="395" t="s">
+        <v>528</v>
+      </c>
+      <c r="V5" s="396" t="s">
+        <v>532</v>
+      </c>
+      <c r="W5" s="398" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
+      <c r="A6" s="394">
+        <v>25</v>
+      </c>
+      <c r="B6" s="395" t="s">
+        <v>567</v>
+      </c>
+      <c r="C6" s="396" t="s">
+        <v>529</v>
+      </c>
+      <c r="D6" s="397" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="398"/>
+      <c r="F6" s="399">
+        <v>19</v>
+      </c>
+      <c r="G6" s="400" t="s">
+        <v>568</v>
+      </c>
+      <c r="H6" s="401"/>
+      <c r="I6" s="402"/>
+      <c r="J6" s="396"/>
+      <c r="K6" s="396"/>
+      <c r="L6" s="399" t="s">
         <v>531</v>
       </c>
-      <c r="V5" s="520" t="s">
-        <v>535</v>
-      </c>
-      <c r="W5" s="522" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" s="11" customFormat="1">
-      <c r="A6" s="518">
-        <v>25</v>
-      </c>
-      <c r="B6" s="519" t="s">
-        <v>570</v>
-      </c>
-      <c r="C6" s="520" t="s">
-        <v>532</v>
-      </c>
-      <c r="D6" s="521" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="522"/>
-      <c r="F6" s="523">
-        <v>19</v>
-      </c>
-      <c r="G6" s="524" t="s">
-        <v>571</v>
-      </c>
-      <c r="H6" s="525"/>
-      <c r="I6" s="526"/>
-      <c r="J6" s="520"/>
-      <c r="K6" s="520"/>
-      <c r="L6" s="523" t="s">
-        <v>534</v>
-      </c>
-      <c r="M6" s="525"/>
-      <c r="N6" s="525"/>
-      <c r="O6" s="527"/>
+      <c r="M6" s="401"/>
+      <c r="N6" s="401"/>
+      <c r="O6" s="403"/>
       <c r="P6" s="11" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="Q6" s="11" t="e">
         <v>#N/A</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="S6" s="11" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T6" s="518">
+      <c r="T6" s="394">
         <v>25</v>
       </c>
-      <c r="U6" s="519" t="s">
-        <v>570</v>
-      </c>
-      <c r="V6" s="520" t="s">
-        <v>532</v>
-      </c>
-      <c r="W6" s="522" t="s">
+      <c r="U6" s="395" t="s">
+        <v>567</v>
+      </c>
+      <c r="V6" s="396" t="s">
+        <v>529</v>
+      </c>
+      <c r="W6" s="398" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="11" customFormat="1">
-      <c r="A7" s="518">
+    <row r="7" spans="1:23">
+      <c r="A7" s="394">
         <v>54</v>
       </c>
-      <c r="B7" s="519" t="s">
+      <c r="B7" s="395" t="s">
+        <v>574</v>
+      </c>
+      <c r="C7" s="396" t="s">
+        <v>575</v>
+      </c>
+      <c r="D7" s="397" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="398"/>
+      <c r="F7" s="399" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="400" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="397">
+        <v>3</v>
+      </c>
+      <c r="I7" s="402" t="s">
+        <v>535</v>
+      </c>
+      <c r="J7" s="398" t="s">
+        <v>537</v>
+      </c>
+      <c r="K7" s="405" t="s">
+        <v>576</v>
+      </c>
+      <c r="L7" s="399" t="s">
+        <v>531</v>
+      </c>
+      <c r="M7" s="397"/>
+      <c r="N7" s="397"/>
+      <c r="O7" s="404"/>
+      <c r="P7" s="11" t="s">
         <v>577</v>
       </c>
-      <c r="C7" s="520" t="s">
-        <v>578</v>
-      </c>
-      <c r="D7" s="521" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="522"/>
-      <c r="F7" s="523" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="524" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="521">
-        <v>3</v>
-      </c>
-      <c r="I7" s="526" t="s">
-        <v>538</v>
-      </c>
-      <c r="J7" s="522" t="s">
-        <v>540</v>
-      </c>
-      <c r="K7" s="529" t="s">
-        <v>579</v>
-      </c>
-      <c r="L7" s="523" t="s">
-        <v>534</v>
-      </c>
-      <c r="M7" s="521"/>
-      <c r="N7" s="521"/>
-      <c r="O7" s="528"/>
-      <c r="P7" s="11" t="s">
-        <v>580</v>
-      </c>
       <c r="Q7" s="11" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="R7" s="11" t="e">
         <v>#N/A</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>580</v>
-      </c>
-      <c r="T7" s="518">
+        <v>577</v>
+      </c>
+      <c r="T7" s="394">
         <v>54</v>
       </c>
-      <c r="U7" s="519" t="s">
-        <v>577</v>
-      </c>
-      <c r="V7" s="520" t="s">
+      <c r="U7" s="395" t="s">
+        <v>574</v>
+      </c>
+      <c r="V7" s="396" t="s">
+        <v>575</v>
+      </c>
+      <c r="W7" s="398" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8" s="394">
+        <v>54</v>
+      </c>
+      <c r="B8" s="395" t="s">
+        <v>574</v>
+      </c>
+      <c r="C8" s="396" t="s">
+        <v>575</v>
+      </c>
+      <c r="D8" s="397" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="398"/>
+      <c r="F8" s="399" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="400" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="397">
+        <v>4</v>
+      </c>
+      <c r="I8" s="402" t="s">
+        <v>540</v>
+      </c>
+      <c r="J8" s="398" t="s">
+        <v>537</v>
+      </c>
+      <c r="K8" s="405" t="s">
+        <v>576</v>
+      </c>
+      <c r="L8" s="399" t="s">
+        <v>531</v>
+      </c>
+      <c r="M8" s="397"/>
+      <c r="N8" s="397"/>
+      <c r="O8" s="404"/>
+      <c r="P8" s="11" t="s">
         <v>578</v>
       </c>
-      <c r="W7" s="522" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" s="11" customFormat="1">
-      <c r="A8" s="518">
-        <v>54</v>
-      </c>
-      <c r="B8" s="519" t="s">
-        <v>577</v>
-      </c>
-      <c r="C8" s="520" t="s">
+      <c r="Q8" s="11" t="s">
         <v>578</v>
-      </c>
-      <c r="D8" s="521" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="522"/>
-      <c r="F8" s="523" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="524" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="521">
-        <v>4</v>
-      </c>
-      <c r="I8" s="526" t="s">
-        <v>543</v>
-      </c>
-      <c r="J8" s="522" t="s">
-        <v>540</v>
-      </c>
-      <c r="K8" s="529" t="s">
-        <v>579</v>
-      </c>
-      <c r="L8" s="523" t="s">
-        <v>534</v>
-      </c>
-      <c r="M8" s="521"/>
-      <c r="N8" s="521"/>
-      <c r="O8" s="528"/>
-      <c r="P8" s="11" t="s">
-        <v>581</v>
-      </c>
-      <c r="Q8" s="11" t="s">
-        <v>581</v>
       </c>
       <c r="R8" s="11" t="e">
         <v>#N/A</v>
       </c>
       <c r="S8" s="11" t="s">
-        <v>581</v>
-      </c>
-      <c r="T8" s="518">
+        <v>578</v>
+      </c>
+      <c r="T8" s="394">
         <v>54</v>
       </c>
-      <c r="U8" s="519" t="s">
-        <v>577</v>
-      </c>
-      <c r="V8" s="520" t="s">
-        <v>578</v>
-      </c>
-      <c r="W8" s="522" t="s">
+      <c r="U8" s="395" t="s">
+        <v>574</v>
+      </c>
+      <c r="V8" s="396" t="s">
+        <v>575</v>
+      </c>
+      <c r="W8" s="398" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="9" spans="1:23">
+      <c r="A9" s="394">
+        <v>25</v>
+      </c>
+      <c r="B9" s="395" t="s">
+        <v>567</v>
+      </c>
+      <c r="C9" s="396" t="s">
+        <v>529</v>
+      </c>
+      <c r="D9" s="397" t="s">
+        <v>607</v>
+      </c>
+      <c r="E9" s="398" t="s">
+        <v>608</v>
+      </c>
+      <c r="F9" s="399">
+        <v>19</v>
+      </c>
+      <c r="G9" s="400" t="s">
+        <v>568</v>
+      </c>
+      <c r="H9" s="464"/>
+      <c r="I9" s="402"/>
+      <c r="J9" s="396"/>
+      <c r="K9" s="396"/>
+      <c r="L9" s="399" t="s">
+        <v>531</v>
+      </c>
+      <c r="M9" s="401"/>
+      <c r="N9" s="401"/>
+      <c r="O9" s="403"/>
+      <c r="P9" s="11" t="s">
+        <v>609</v>
+      </c>
+      <c r="Q9" s="394">
+        <v>25</v>
+      </c>
+      <c r="R9" s="395" t="s">
+        <v>567</v>
+      </c>
+      <c r="S9" s="396" t="s">
+        <v>529</v>
+      </c>
+      <c r="T9" s="394">
+        <v>25</v>
+      </c>
+      <c r="U9" s="395" t="s">
+        <v>567</v>
+      </c>
+      <c r="V9" s="396" t="s">
+        <v>529</v>
+      </c>
+      <c r="W9" s="398" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10" s="394">
+        <v>55</v>
+      </c>
+      <c r="B10" s="395" t="s">
+        <v>610</v>
+      </c>
+      <c r="C10" s="396" t="s">
+        <v>529</v>
+      </c>
+      <c r="D10" s="397" t="s">
+        <v>611</v>
+      </c>
+      <c r="E10" s="398" t="s">
+        <v>612</v>
+      </c>
+      <c r="F10" s="399">
+        <v>12</v>
+      </c>
+      <c r="G10" s="400" t="s">
+        <v>613</v>
+      </c>
+      <c r="H10" s="464"/>
+      <c r="I10" s="402"/>
+      <c r="J10" s="396"/>
+      <c r="K10" s="396"/>
+      <c r="L10" s="399" t="s">
+        <v>531</v>
+      </c>
+      <c r="M10" s="401"/>
+      <c r="N10" s="401"/>
+      <c r="O10" s="403"/>
+      <c r="P10" s="11" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q10" s="394">
+        <v>55</v>
+      </c>
+      <c r="R10" s="395" t="s">
+        <v>610</v>
+      </c>
+      <c r="S10" s="396" t="s">
+        <v>529</v>
+      </c>
+      <c r="T10" s="394">
+        <v>55</v>
+      </c>
+      <c r="U10" s="395" t="s">
+        <v>610</v>
+      </c>
+      <c r="V10" s="396" t="s">
+        <v>529</v>
+      </c>
+      <c r="W10" s="398" t="s">
+        <v>611</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:W1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="142" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
@@ -34017,215 +34213,215 @@
       </c>
       <c r="X1" s="49"/>
       <c r="Z1" s="49"/>
-      <c r="AA1" s="509" t="s">
+      <c r="AA1" s="580" t="s">
         <v>176</v>
       </c>
-      <c r="AB1" s="510"/>
-      <c r="AC1" s="511" t="s">
+      <c r="AB1" s="581"/>
+      <c r="AC1" s="582" t="s">
         <v>107</v>
       </c>
-      <c r="AD1" s="511"/>
-      <c r="AE1" s="511"/>
-      <c r="AF1" s="511"/>
-      <c r="AG1" s="511"/>
-      <c r="AH1" s="511"/>
-      <c r="AI1" s="511"/>
-      <c r="AJ1" s="512"/>
-      <c r="AK1" s="513" t="s">
+      <c r="AD1" s="582"/>
+      <c r="AE1" s="582"/>
+      <c r="AF1" s="582"/>
+      <c r="AG1" s="582"/>
+      <c r="AH1" s="582"/>
+      <c r="AI1" s="582"/>
+      <c r="AJ1" s="583"/>
+      <c r="AK1" s="584" t="s">
         <v>178</v>
       </c>
-      <c r="AL1" s="514"/>
-      <c r="AM1" s="514"/>
-      <c r="AN1" s="514"/>
-      <c r="AO1" s="514"/>
-      <c r="AP1" s="514"/>
-      <c r="AQ1" s="514"/>
-      <c r="AR1" s="515" t="s">
+      <c r="AL1" s="585"/>
+      <c r="AM1" s="585"/>
+      <c r="AN1" s="585"/>
+      <c r="AO1" s="585"/>
+      <c r="AP1" s="585"/>
+      <c r="AQ1" s="585"/>
+      <c r="AR1" s="586" t="s">
         <v>187</v>
       </c>
-      <c r="AS1" s="516"/>
-      <c r="AT1" s="516"/>
-      <c r="AU1" s="516"/>
-      <c r="AV1" s="516"/>
-      <c r="AW1" s="516"/>
-      <c r="AX1" s="516"/>
-      <c r="AY1" s="516"/>
-      <c r="AZ1" s="515" t="s">
+      <c r="AS1" s="587"/>
+      <c r="AT1" s="587"/>
+      <c r="AU1" s="587"/>
+      <c r="AV1" s="587"/>
+      <c r="AW1" s="587"/>
+      <c r="AX1" s="587"/>
+      <c r="AY1" s="587"/>
+      <c r="AZ1" s="586" t="s">
         <v>188</v>
       </c>
-      <c r="BA1" s="516"/>
-      <c r="BB1" s="516"/>
-      <c r="BC1" s="517"/>
-      <c r="BD1" s="498" t="s">
+      <c r="BA1" s="587"/>
+      <c r="BB1" s="587"/>
+      <c r="BC1" s="588"/>
+      <c r="BD1" s="569" t="s">
         <v>2</v>
       </c>
-      <c r="BE1" s="499"/>
-      <c r="BF1" s="499"/>
-      <c r="BG1" s="499"/>
-      <c r="BH1" s="499"/>
-      <c r="BI1" s="500"/>
-      <c r="BJ1" s="501"/>
-      <c r="BK1" s="502" t="s">
+      <c r="BE1" s="570"/>
+      <c r="BF1" s="570"/>
+      <c r="BG1" s="570"/>
+      <c r="BH1" s="570"/>
+      <c r="BI1" s="571"/>
+      <c r="BJ1" s="572"/>
+      <c r="BK1" s="573" t="s">
         <v>3</v>
       </c>
-      <c r="BL1" s="503"/>
-      <c r="BM1" s="503"/>
-      <c r="BN1" s="504" t="s">
+      <c r="BL1" s="574"/>
+      <c r="BM1" s="574"/>
+      <c r="BN1" s="575" t="s">
         <v>4</v>
       </c>
-      <c r="BO1" s="505"/>
-      <c r="BP1" s="505"/>
-      <c r="BQ1" s="505"/>
-      <c r="BR1" s="505"/>
-      <c r="BS1" s="506"/>
-      <c r="BT1" s="506"/>
-      <c r="BU1" s="506"/>
-      <c r="BV1" s="507" t="s">
+      <c r="BO1" s="576"/>
+      <c r="BP1" s="576"/>
+      <c r="BQ1" s="576"/>
+      <c r="BR1" s="576"/>
+      <c r="BS1" s="577"/>
+      <c r="BT1" s="577"/>
+      <c r="BU1" s="577"/>
+      <c r="BV1" s="578" t="s">
         <v>5</v>
       </c>
-      <c r="BW1" s="508"/>
-      <c r="BX1" s="486" t="s">
+      <c r="BW1" s="579"/>
+      <c r="BX1" s="557" t="s">
         <v>164</v>
       </c>
-      <c r="BY1" s="487"/>
-      <c r="BZ1" s="488"/>
-      <c r="CA1" s="489" t="s">
+      <c r="BY1" s="558"/>
+      <c r="BZ1" s="559"/>
+      <c r="CA1" s="560" t="s">
         <v>165</v>
       </c>
-      <c r="CB1" s="490"/>
-      <c r="CC1" s="491" t="s">
+      <c r="CB1" s="561"/>
+      <c r="CC1" s="562" t="s">
         <v>6</v>
       </c>
-      <c r="CD1" s="492"/>
-      <c r="CE1" s="493"/>
-      <c r="CF1" s="494" t="s">
+      <c r="CD1" s="563"/>
+      <c r="CE1" s="564"/>
+      <c r="CF1" s="565" t="s">
         <v>166</v>
       </c>
-      <c r="CG1" s="495"/>
-      <c r="CH1" s="495"/>
-      <c r="CI1" s="496" t="s">
+      <c r="CG1" s="566"/>
+      <c r="CH1" s="566"/>
+      <c r="CI1" s="567" t="s">
         <v>167</v>
       </c>
-      <c r="CJ1" s="497"/>
-      <c r="CK1" s="497"/>
-      <c r="CL1" s="457" t="s">
+      <c r="CJ1" s="568"/>
+      <c r="CK1" s="568"/>
+      <c r="CL1" s="528" t="s">
         <v>168</v>
       </c>
-      <c r="CM1" s="458"/>
-      <c r="CN1" s="458"/>
-      <c r="CO1" s="458"/>
-      <c r="CP1" s="458"/>
-      <c r="CQ1" s="459" t="s">
+      <c r="CM1" s="529"/>
+      <c r="CN1" s="529"/>
+      <c r="CO1" s="529"/>
+      <c r="CP1" s="529"/>
+      <c r="CQ1" s="530" t="s">
         <v>169</v>
       </c>
-      <c r="CR1" s="460"/>
-      <c r="CS1" s="461"/>
-      <c r="CT1" s="462" t="s">
+      <c r="CR1" s="531"/>
+      <c r="CS1" s="532"/>
+      <c r="CT1" s="533" t="s">
         <v>170</v>
       </c>
-      <c r="CU1" s="463"/>
-      <c r="CV1" s="463"/>
-      <c r="CW1" s="464"/>
-      <c r="CX1" s="464"/>
-      <c r="CY1" s="464"/>
-      <c r="CZ1" s="465"/>
-      <c r="DA1" s="469" t="s">
+      <c r="CU1" s="534"/>
+      <c r="CV1" s="534"/>
+      <c r="CW1" s="535"/>
+      <c r="CX1" s="535"/>
+      <c r="CY1" s="535"/>
+      <c r="CZ1" s="536"/>
+      <c r="DA1" s="540" t="s">
         <v>198</v>
       </c>
-      <c r="DB1" s="470"/>
-      <c r="DC1" s="476" t="s">
+      <c r="DB1" s="541"/>
+      <c r="DC1" s="547" t="s">
         <v>199</v>
       </c>
-      <c r="DD1" s="477"/>
-      <c r="DE1" s="478"/>
-      <c r="DF1" s="476" t="s">
+      <c r="DD1" s="548"/>
+      <c r="DE1" s="549"/>
+      <c r="DF1" s="547" t="s">
         <v>7</v>
       </c>
-      <c r="DG1" s="478"/>
-      <c r="DH1" s="479" t="s">
+      <c r="DG1" s="549"/>
+      <c r="DH1" s="550" t="s">
         <v>171</v>
       </c>
-      <c r="DI1" s="480"/>
-      <c r="DJ1" s="481" t="s">
+      <c r="DI1" s="551"/>
+      <c r="DJ1" s="552" t="s">
         <v>172</v>
       </c>
-      <c r="DK1" s="482"/>
-      <c r="DL1" s="483"/>
+      <c r="DK1" s="553"/>
+      <c r="DL1" s="554"/>
       <c r="DM1" s="73" t="s">
         <v>173</v>
       </c>
-      <c r="DN1" s="471" t="s">
+      <c r="DN1" s="542" t="s">
         <v>174</v>
       </c>
-      <c r="DO1" s="472"/>
-      <c r="DP1" s="473"/>
-      <c r="DQ1" s="484" t="s">
+      <c r="DO1" s="543"/>
+      <c r="DP1" s="544"/>
+      <c r="DQ1" s="555" t="s">
         <v>200</v>
       </c>
-      <c r="DR1" s="485"/>
-      <c r="DS1" s="485"/>
+      <c r="DR1" s="556"/>
+      <c r="DS1" s="556"/>
       <c r="DT1" s="74" t="s">
         <v>201</v>
       </c>
-      <c r="DU1" s="474" t="s">
+      <c r="DU1" s="545" t="s">
         <v>202</v>
       </c>
-      <c r="DV1" s="475"/>
-      <c r="DW1" s="475"/>
-      <c r="DX1" s="466" t="s">
+      <c r="DV1" s="546"/>
+      <c r="DW1" s="546"/>
+      <c r="DX1" s="537" t="s">
         <v>203</v>
       </c>
-      <c r="DY1" s="467"/>
-      <c r="DZ1" s="468"/>
+      <c r="DY1" s="538"/>
+      <c r="DZ1" s="539"/>
     </row>
     <row r="2" spans="1:130" s="14" customFormat="1" ht="79.5" thickBot="1">
       <c r="A2" s="393" t="s">
+        <v>506</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>507</v>
+      </c>
+      <c r="C2" s="52" t="s">
+        <v>508</v>
+      </c>
+      <c r="D2" s="52" t="s">
         <v>509</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="E2" s="70" t="s">
         <v>510</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="F2" s="82" t="s">
         <v>511</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="G2" s="70" t="s">
         <v>512</v>
       </c>
-      <c r="E2" s="70" t="s">
+      <c r="H2" s="82" t="s">
         <v>513</v>
       </c>
-      <c r="F2" s="82" t="s">
+      <c r="I2" s="70" t="s">
         <v>514</v>
-      </c>
-      <c r="G2" s="70" t="s">
-        <v>515</v>
-      </c>
-      <c r="H2" s="82" t="s">
-        <v>516</v>
-      </c>
-      <c r="I2" s="70" t="s">
-        <v>517</v>
       </c>
       <c r="J2" s="82" t="s">
         <v>497</v>
       </c>
       <c r="K2" s="82" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="L2" s="70" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="M2" s="70" t="s">
+        <v>515</v>
+      </c>
+      <c r="N2" s="70" t="s">
+        <v>516</v>
+      </c>
+      <c r="O2" s="82" t="s">
+        <v>517</v>
+      </c>
+      <c r="P2" s="82" t="s">
         <v>518</v>
-      </c>
-      <c r="N2" s="70" t="s">
-        <v>519</v>
-      </c>
-      <c r="O2" s="82" t="s">
-        <v>520</v>
-      </c>
-      <c r="P2" s="82" t="s">
-        <v>521</v>
       </c>
       <c r="Q2" s="372" t="s">
         <v>479</v>

</xml_diff>